<commit_message>
change to override https://github.com/zenodo/zenodo/issues/2478
</commit_message>
<xml_diff>
--- a/qPCR/input/Table_combinedInputs.xlsx
+++ b/qPCR/input/Table_combinedInputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majaz\Desktop\backup\GitHub\Bacillus-Pti5\qPCR\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EF010A-1854-493F-B63E-7F97A1912BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9918FC-298C-47A3-B023-740404D4BA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="790" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="790" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S1_PrimerTable" sheetId="19" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2572" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="602">
   <si>
     <t>Functional group</t>
   </si>
@@ -2135,6 +2135,48 @@
   </si>
   <si>
     <t>Expression of selected potato genes after mycorrhizal colonization.</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>BS1013</t>
+  </si>
+  <si>
+    <t>BS1021</t>
+  </si>
+  <si>
+    <t>BS1029</t>
+  </si>
+  <si>
+    <t>BS1037</t>
+  </si>
+  <si>
+    <t>BS1045</t>
+  </si>
+  <si>
+    <t>apex+ 2 leaves</t>
+  </si>
+  <si>
+    <t>BS1053</t>
+  </si>
+  <si>
+    <t>BS1061</t>
+  </si>
+  <si>
+    <t>BS1069</t>
+  </si>
+  <si>
+    <t>apex+ 4th leave+nodes and internodes</t>
+  </si>
+  <si>
+    <t>BS1085</t>
+  </si>
+  <si>
+    <t>BS1077</t>
+  </si>
+  <si>
+    <t>apex+4th leave+nodes and internodes</t>
   </si>
 </sst>
 </file>
@@ -2807,7 +2849,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3282,6 +3324,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4348,10 +4395,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F000CA-C4A3-4DEE-ADD6-1092CD5E1D6A}">
-  <dimension ref="A1:T52"/>
+  <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4567,948 +4614,1178 @@
       <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="153" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" s="202" t="s">
+        <v>339</v>
+      </c>
+      <c r="C11" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D11" s="153" t="s">
+        <v>340</v>
+      </c>
+      <c r="E11" s="202" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="203" t="s">
+        <v>588</v>
+      </c>
+      <c r="K11" s="28"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="153" t="s">
+        <v>354</v>
+      </c>
+      <c r="B12" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C12" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D12" s="153" t="s">
+        <v>342</v>
+      </c>
+      <c r="E12" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="153" t="s">
+        <v>360</v>
+      </c>
+      <c r="B13" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C13" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D13" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="E13" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="153" t="s">
+        <v>362</v>
+      </c>
+      <c r="B14" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C14" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D14" s="153" t="s">
+        <v>363</v>
+      </c>
+      <c r="E14" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="153" t="s">
+        <v>365</v>
+      </c>
+      <c r="B15" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C15" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D15" s="153" t="s">
+        <v>366</v>
+      </c>
+      <c r="E15" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="153" t="s">
+        <v>369</v>
+      </c>
+      <c r="B16" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C16" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D16" s="153" t="s">
+        <v>346</v>
+      </c>
+      <c r="E16" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="153" t="s">
+        <v>589</v>
+      </c>
+      <c r="B17" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C17" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D17" s="153" t="s">
+        <v>399</v>
+      </c>
+      <c r="E17" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="153" t="s">
+        <v>352</v>
+      </c>
+      <c r="B18" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C18" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D18" s="153" t="s">
+        <v>340</v>
+      </c>
+      <c r="E18" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="153" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="153" t="s">
+        <v>355</v>
+      </c>
+      <c r="B19" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C19" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D19" s="153" t="s">
+        <v>342</v>
+      </c>
+      <c r="E19" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="153" t="s">
+        <v>358</v>
+      </c>
+      <c r="B20" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C20" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D20" s="153" t="s">
+        <v>359</v>
+      </c>
+      <c r="E20" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="153" t="s">
+        <v>364</v>
+      </c>
+      <c r="B21" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C21" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D21" s="153" t="s">
+        <v>363</v>
+      </c>
+      <c r="E21" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="153" t="s">
+        <v>367</v>
+      </c>
+      <c r="B22" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C22" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D22" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="E22" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="153" t="s">
+        <v>590</v>
+      </c>
+      <c r="B23" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C23" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D23" s="153" t="s">
+        <v>399</v>
+      </c>
+      <c r="E23" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="153" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="153" t="s">
+        <v>356</v>
+      </c>
+      <c r="B24" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C24" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D24" s="153" t="s">
+        <v>330</v>
+      </c>
+      <c r="E24" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="153" t="s">
+        <v>361</v>
+      </c>
+      <c r="B25" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C25" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D25" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="E25" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="153" t="s">
+        <v>368</v>
+      </c>
+      <c r="B26" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C26" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D26" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="E26" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="153" t="s">
+        <v>370</v>
+      </c>
+      <c r="B27" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C27" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D27" s="153" t="s">
+        <v>346</v>
+      </c>
+      <c r="E27" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="153" t="s">
+        <v>591</v>
+      </c>
+      <c r="B28" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C28" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D28" s="153" t="s">
+        <v>399</v>
+      </c>
+      <c r="E28" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" s="153" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="153" t="s">
+        <v>347</v>
+      </c>
+      <c r="B29" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C29" s="153" t="s">
+        <v>348</v>
+      </c>
+      <c r="D29" s="153" t="s">
+        <v>349</v>
+      </c>
+      <c r="E29" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="204" t="s">
+        <v>592</v>
+      </c>
+      <c r="B30" s="204" t="s">
+        <v>339</v>
+      </c>
+      <c r="C30" s="204" t="s">
+        <v>348</v>
+      </c>
+      <c r="D30" s="204" t="s">
+        <v>399</v>
+      </c>
+      <c r="E30" s="204" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="204" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="204" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="153" t="s">
+        <v>376</v>
+      </c>
+      <c r="B31" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D31" s="153" t="s">
+        <v>330</v>
+      </c>
+      <c r="E31" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="153" t="s">
+        <v>378</v>
+      </c>
+      <c r="B32" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D32" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="E32" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="153" t="s">
+        <v>384</v>
+      </c>
+      <c r="B33" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D33" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="E33" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="203" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="153" t="s">
+        <v>386</v>
+      </c>
+      <c r="B34" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D34" s="153" t="s">
+        <v>346</v>
+      </c>
+      <c r="E34" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="153" t="s">
+        <v>593</v>
+      </c>
+      <c r="B35" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D35" s="153" t="s">
+        <v>594</v>
+      </c>
+      <c r="E35" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" s="203" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="153" t="s">
+        <v>371</v>
+      </c>
+      <c r="B36" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D36" s="153" t="s">
+        <v>340</v>
+      </c>
+      <c r="E36" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="153" t="s">
+        <v>373</v>
+      </c>
+      <c r="B37" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D37" s="153" t="s">
+        <v>342</v>
+      </c>
+      <c r="E37" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="153" t="s">
+        <v>379</v>
+      </c>
+      <c r="B38" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D38" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="E38" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="153" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="153" t="s">
+        <v>383</v>
+      </c>
+      <c r="B39" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D39" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="E39" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G39" s="153" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="153" t="s">
+        <v>387</v>
+      </c>
+      <c r="B40" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D40" s="153" t="s">
+        <v>346</v>
+      </c>
+      <c r="E40" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" s="203" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="153" t="s">
+        <v>595</v>
+      </c>
+      <c r="B41" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D41" s="153" t="s">
+        <v>399</v>
+      </c>
+      <c r="E41" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="153" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="153" t="s">
+        <v>372</v>
+      </c>
+      <c r="B42" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D42" s="153" t="s">
+        <v>340</v>
+      </c>
+      <c r="E42" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F42" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="153" t="s">
+        <v>374</v>
+      </c>
+      <c r="B43" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D43" s="153" t="s">
+        <v>342</v>
+      </c>
+      <c r="E43" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G43" s="153" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="153" t="s">
+        <v>380</v>
+      </c>
+      <c r="B44" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D44" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="E44" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" s="203" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="153" t="s">
+        <v>382</v>
+      </c>
+      <c r="B45" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D45" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="E45" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" s="203" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="153" t="s">
+        <v>388</v>
+      </c>
+      <c r="B46" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D46" s="153" t="s">
+        <v>346</v>
+      </c>
+      <c r="E46" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F46" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G46" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="153" t="s">
+        <v>596</v>
+      </c>
+      <c r="B47" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="153" t="s">
+        <v>357</v>
+      </c>
+      <c r="D47" s="153" t="s">
+        <v>399</v>
+      </c>
+      <c r="E47" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G47" s="203" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="153" t="s">
+        <v>377</v>
+      </c>
+      <c r="B48" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="153" t="s">
+        <v>348</v>
+      </c>
+      <c r="D48" s="153" t="s">
+        <v>330</v>
+      </c>
+      <c r="E48" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F48" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="153" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="153" t="s">
+        <v>381</v>
+      </c>
+      <c r="B49" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="153" t="s">
+        <v>348</v>
+      </c>
+      <c r="D49" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="E49" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F49" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G49" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="153" t="s">
+        <v>385</v>
+      </c>
+      <c r="B50" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="153" t="s">
+        <v>348</v>
+      </c>
+      <c r="D50" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="E50" s="153" t="s">
+        <v>103</v>
+      </c>
+      <c r="F50" s="153" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="203" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="204" t="s">
+        <v>597</v>
+      </c>
+      <c r="B51" s="204" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="204" t="s">
+        <v>348</v>
+      </c>
+      <c r="D51" s="204" t="s">
+        <v>598</v>
+      </c>
+      <c r="E51" s="204" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="204" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" s="205" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="153" t="s">
+        <v>338</v>
+      </c>
+      <c r="B52" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C52" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D52" s="153" t="s">
+        <v>340</v>
+      </c>
+      <c r="E52" s="153" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="203"/>
+      <c r="G52" s="153" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="153" t="s">
+        <v>341</v>
+      </c>
+      <c r="B53" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C53" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D53" s="153" t="s">
+        <v>342</v>
+      </c>
+      <c r="E53" s="153" t="s">
+        <v>98</v>
+      </c>
+      <c r="F53" s="203"/>
+      <c r="G53" s="153" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="153" t="s">
+        <v>343</v>
+      </c>
+      <c r="B54" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C54" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D54" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="E54" s="153" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54" s="203"/>
+      <c r="G54" s="153" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="153" t="s">
+        <v>344</v>
+      </c>
+      <c r="B55" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C55" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D55" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="E55" s="153" t="s">
+        <v>98</v>
+      </c>
+      <c r="F55" s="203"/>
+      <c r="G55" s="153" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="153" t="s">
+        <v>345</v>
+      </c>
+      <c r="B56" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C56" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D56" s="153" t="s">
+        <v>346</v>
+      </c>
+      <c r="E56" s="153" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" s="203"/>
+      <c r="G56" s="153" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="153" t="s">
+        <v>599</v>
+      </c>
+      <c r="B57" s="153" t="s">
+        <v>339</v>
+      </c>
+      <c r="C57" s="153" t="s">
+        <v>326</v>
+      </c>
+      <c r="D57" s="153" t="s">
+        <v>399</v>
+      </c>
+      <c r="E57" s="153" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" s="203"/>
+      <c r="G57" s="153" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="204" t="s">
+        <v>600</v>
+      </c>
+      <c r="B58" s="204" t="s">
+        <v>339</v>
+      </c>
+      <c r="C58" s="204" t="s">
+        <v>326</v>
+      </c>
+      <c r="D58" s="204" t="s">
+        <v>601</v>
+      </c>
+      <c r="E58" s="204" t="s">
+        <v>98</v>
+      </c>
+      <c r="F58" s="205"/>
+      <c r="G58" s="204" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="153" t="s">
         <v>329</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B59" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="153" t="s">
         <v>326</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D59" s="153" t="s">
         <v>330</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E59" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="4" t="s">
+      <c r="F59" s="206"/>
+      <c r="G59" s="153" t="s">
         <v>331</v>
       </c>
-      <c r="K11" s="28"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="4" t="s">
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="153" t="s">
         <v>332</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B60" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="153" t="s">
         <v>326</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D60" s="153" t="s">
         <v>333</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E60" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="4" t="s">
+      <c r="F60" s="206"/>
+      <c r="G60" s="153" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="4" t="s">
+    <row r="61" spans="1:7">
+      <c r="A61" s="153" t="s">
         <v>335</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B61" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="153" t="s">
         <v>326</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D61" s="153" t="s">
         <v>333</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E61" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="4" t="s">
+      <c r="F61" s="206"/>
+      <c r="G61" s="153" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="4" t="s">
+    <row r="62" spans="1:7">
+      <c r="A62" s="153" t="s">
         <v>336</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B62" s="153" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="153" t="s">
         <v>326</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D62" s="153" t="s">
         <v>337</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E62" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="4" t="s">
+      <c r="F62" s="206"/>
+      <c r="G62" s="153" t="s">
         <v>334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="10" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G21" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G24" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G25" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G26" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G27" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G28" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G29" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G30" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G31" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G33" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G34" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G36" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G38" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G39" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G40" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G41" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G42" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G43" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G44" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G45" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G46" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G47" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G48" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G49" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G51" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G52" t="s">
-        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5523,7 +5800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF70B9E2-5338-47B7-8847-74CB1F09AEF3}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -8491,7 +8768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B72514D-98CA-4FEB-8DF4-C87BC09EF3E2}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -21784,14 +22061,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b6814e5f-7717-498d-b3f9-a579343416c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6e8d83df-c883-47f3-baec-2c3f36f86628" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22036,27 +22311,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b6814e5f-7717-498d-b3f9-a579343416c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6e8d83df-c883-47f3-baec-2c3f36f86628" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A56411B5-B9A9-4470-84DC-F755F2F8BA09}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E47AE928-FFC5-4E41-90D6-BE7C2F0E55F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6e8d83df-c883-47f3-baec-2c3f36f86628"/>
-    <ds:schemaRef ds:uri="b6814e5f-7717-498d-b3f9-a579343416c6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22081,9 +22349,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E47AE928-FFC5-4E41-90D6-BE7C2F0E55F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A56411B5-B9A9-4470-84DC-F755F2F8BA09}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6e8d83df-c883-47f3-baec-2c3f36f86628"/>
+    <ds:schemaRef ds:uri="b6814e5f-7717-498d-b3f9-a579343416c6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>